<commit_message>
Feito o importador com repetição
/spend 4h
</commit_message>
<xml_diff>
--- a/tests/Modelo-tse-extendido.xlsx
+++ b/tests/Modelo-tse-extendido.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">UP</t>
   </si>
   <si>
-    <t xml:space="preserve">Regular</t>
+    <t xml:space="preserve">REGULAR</t>
   </si>
   <si>
     <t xml:space="preserve">N�o</t>
@@ -253,6 +253,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -336,20 +337,20 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3:I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.22"/>
   </cols>

</xml_diff>